<commit_message>
needs small css touches and upload to delsol only
</commit_message>
<xml_diff>
--- a/server/basePresupuestosExcel.xlsx
+++ b/server/basePresupuestosExcel.xlsx
@@ -970,7 +970,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="227">
+  <cellXfs count="226">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1237,8 +1237,6 @@
     <xf numFmtId="0" fontId="44" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1253,20 +1251,35 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="45" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="4" fontId="45" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="4" fontId="45" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="4" fontId="45" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2284,7 +2297,7 @@
   <dimension ref="B3:J65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="B18" sqref="B18:F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2351,7 +2364,7 @@
       <c r="D9" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="210"/>
+      <c r="E9" s="208"/>
       <c r="F9" s="25"/>
       <c r="J9" s="67"/>
     </row>
@@ -2359,12 +2372,12 @@
       <c r="B10" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="215"/>
-      <c r="D10" s="215" t="s">
+      <c r="C10" s="213"/>
+      <c r="D10" s="213" t="s">
         <v>19</v>
       </c>
       <c r="E10" s="53"/>
-      <c r="F10" s="212"/>
+      <c r="F10" s="210"/>
       <c r="I10"/>
       <c r="J10" s="67"/>
     </row>
@@ -2372,14 +2385,14 @@
       <c r="B11" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="217" t="s">
+      <c r="C11" s="215" t="s">
         <v>118</v>
       </c>
-      <c r="D11" s="217" t="s">
+      <c r="D11" s="215" t="s">
         <v>20</v>
       </c>
       <c r="E11" s="202"/>
-      <c r="F11" s="214"/>
+      <c r="F11" s="212"/>
       <c r="I11"/>
       <c r="J11" s="67"/>
     </row>
@@ -2387,22 +2400,22 @@
       <c r="B12" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="215"/>
-      <c r="D12" s="215" t="s">
+      <c r="C12" s="213"/>
+      <c r="D12" s="213" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="216"/>
-      <c r="F12" s="212"/>
+      <c r="E12" s="214"/>
+      <c r="F12" s="210"/>
       <c r="I12"/>
     </row>
     <row r="13" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B13" s="215" t="s">
+      <c r="B13" s="213" t="s">
         <v>111</v>
       </c>
-      <c r="C13" s="211"/>
-      <c r="D13" s="213"/>
-      <c r="E13" s="214"/>
-      <c r="F13" s="214"/>
+      <c r="C13" s="209"/>
+      <c r="D13" s="211"/>
+      <c r="E13" s="212"/>
+      <c r="F13" s="212"/>
       <c r="I13"/>
     </row>
     <row r="14" spans="2:10" ht="23.25" x14ac:dyDescent="0.35">
@@ -2441,11 +2454,11 @@
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="219"/>
-      <c r="C18" s="219"/>
-      <c r="D18" s="219"/>
-      <c r="E18" s="220"/>
-      <c r="F18" s="221" t="str">
+      <c r="B18" s="216"/>
+      <c r="C18" s="216"/>
+      <c r="D18" s="216"/>
+      <c r="E18" s="217"/>
+      <c r="F18" s="217" t="str">
         <f t="shared" ref="F18:F24" si="0">IF(D18&lt;&gt;"",D18*E18,"")</f>
         <v/>
       </c>
@@ -2453,39 +2466,39 @@
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="218"/>
       <c r="C19" s="218"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="221"/>
-      <c r="F19" s="221" t="str">
+      <c r="D19" s="219"/>
+      <c r="E19" s="217"/>
+      <c r="F19" s="217" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="219"/>
+      <c r="B20" s="216"/>
       <c r="C20" s="218"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="221"/>
-      <c r="F20" s="221" t="str">
+      <c r="D20" s="219"/>
+      <c r="E20" s="217"/>
+      <c r="F20" s="217" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="219"/>
+      <c r="B21" s="216"/>
       <c r="C21" s="218"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="221"/>
-      <c r="F21" s="221" t="str">
+      <c r="D21" s="219"/>
+      <c r="E21" s="217"/>
+      <c r="F21" s="217" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="218"/>
-      <c r="C22" s="219"/>
-      <c r="D22" s="219"/>
-      <c r="E22" s="220"/>
-      <c r="F22" s="221" t="str">
+      <c r="C22" s="216"/>
+      <c r="D22" s="216"/>
+      <c r="E22" s="217"/>
+      <c r="F22" s="217" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -2493,19 +2506,19 @@
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="218"/>
       <c r="C23" s="218"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="221"/>
-      <c r="F23" s="221" t="str">
+      <c r="D23" s="219"/>
+      <c r="E23" s="217"/>
+      <c r="F23" s="217" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="219"/>
-      <c r="C24" s="219"/>
-      <c r="D24" s="219"/>
-      <c r="E24" s="220"/>
-      <c r="F24" s="221" t="str">
+      <c r="B24" s="216"/>
+      <c r="C24" s="216"/>
+      <c r="D24" s="216"/>
+      <c r="E24" s="217"/>
+      <c r="F24" s="217" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -2513,19 +2526,19 @@
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="218"/>
       <c r="C25" s="218"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="221"/>
-      <c r="F25" s="221" t="str">
+      <c r="D25" s="219"/>
+      <c r="E25" s="217"/>
+      <c r="F25" s="217" t="str">
         <f>IF(D25&lt;&gt;"",D25*E25,"")</f>
         <v/>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="219"/>
-      <c r="C26" s="219"/>
-      <c r="D26" s="219"/>
-      <c r="E26" s="220"/>
-      <c r="F26" s="221" t="str">
+      <c r="B26" s="216"/>
+      <c r="C26" s="216"/>
+      <c r="D26" s="216"/>
+      <c r="E26" s="217"/>
+      <c r="F26" s="217" t="str">
         <f t="shared" ref="F26:F43" si="1">IF(D26&lt;&gt;"",D26*E26,"")</f>
         <v/>
       </c>
@@ -2534,169 +2547,169 @@
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="218"/>
       <c r="C27" s="218"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="221"/>
-      <c r="F27" s="221" t="str">
+      <c r="D27" s="219"/>
+      <c r="E27" s="217"/>
+      <c r="F27" s="217" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="222"/>
-      <c r="C28" s="223"/>
-      <c r="D28" s="224"/>
-      <c r="E28" s="225"/>
-      <c r="F28" s="221" t="str">
+      <c r="B28" s="220"/>
+      <c r="C28" s="220"/>
+      <c r="D28" s="221"/>
+      <c r="E28" s="222"/>
+      <c r="F28" s="217" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="208"/>
-      <c r="C29" s="208"/>
-      <c r="D29" s="209"/>
-      <c r="E29" s="226"/>
-      <c r="F29" s="221" t="str">
+      <c r="B29" s="223"/>
+      <c r="C29" s="223"/>
+      <c r="D29" s="224"/>
+      <c r="E29" s="222"/>
+      <c r="F29" s="217" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="208"/>
-      <c r="C30" s="208"/>
-      <c r="D30" s="209"/>
-      <c r="E30" s="226"/>
-      <c r="F30" s="221" t="str">
+      <c r="B30" s="223"/>
+      <c r="C30" s="223"/>
+      <c r="D30" s="224"/>
+      <c r="E30" s="222"/>
+      <c r="F30" s="217" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="30"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="221"/>
-      <c r="F31" s="221" t="str">
+      <c r="B31" s="225"/>
+      <c r="C31" s="225"/>
+      <c r="D31" s="219"/>
+      <c r="E31" s="217"/>
+      <c r="F31" s="217" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="30"/>
-      <c r="C32" s="30"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="221"/>
-      <c r="F32" s="221" t="str">
+      <c r="B32" s="225"/>
+      <c r="C32" s="225"/>
+      <c r="D32" s="219"/>
+      <c r="E32" s="217"/>
+      <c r="F32" s="217" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="30"/>
-      <c r="C33" s="30"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="221"/>
-      <c r="F33" s="221" t="str">
+      <c r="B33" s="225"/>
+      <c r="C33" s="225"/>
+      <c r="D33" s="219"/>
+      <c r="E33" s="217"/>
+      <c r="F33" s="217" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="30"/>
-      <c r="C34" s="30"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="221"/>
-      <c r="F34" s="221" t="str">
+      <c r="B34" s="225"/>
+      <c r="C34" s="225"/>
+      <c r="D34" s="219"/>
+      <c r="E34" s="217"/>
+      <c r="F34" s="217" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="30"/>
-      <c r="C35" s="30"/>
-      <c r="D35" s="31"/>
-      <c r="E35" s="221"/>
-      <c r="F35" s="221" t="str">
+      <c r="B35" s="225"/>
+      <c r="C35" s="225"/>
+      <c r="D35" s="219"/>
+      <c r="E35" s="217"/>
+      <c r="F35" s="217" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="30"/>
-      <c r="C36" s="30"/>
-      <c r="D36" s="31"/>
-      <c r="E36" s="221"/>
-      <c r="F36" s="221" t="str">
+      <c r="B36" s="225"/>
+      <c r="C36" s="225"/>
+      <c r="D36" s="219"/>
+      <c r="E36" s="217"/>
+      <c r="F36" s="217" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="30"/>
-      <c r="C37" s="30"/>
-      <c r="D37" s="31"/>
-      <c r="E37" s="221"/>
-      <c r="F37" s="221" t="str">
+      <c r="B37" s="225"/>
+      <c r="C37" s="225"/>
+      <c r="D37" s="219"/>
+      <c r="E37" s="217"/>
+      <c r="F37" s="217" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B38" s="30"/>
-      <c r="C38" s="30"/>
-      <c r="D38" s="31"/>
-      <c r="E38" s="221"/>
-      <c r="F38" s="221" t="str">
+      <c r="B38" s="225"/>
+      <c r="C38" s="225"/>
+      <c r="D38" s="219"/>
+      <c r="E38" s="217"/>
+      <c r="F38" s="217" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B39" s="30"/>
-      <c r="C39" s="30"/>
-      <c r="D39" s="31"/>
-      <c r="E39" s="221"/>
-      <c r="F39" s="221" t="str">
+      <c r="B39" s="225"/>
+      <c r="C39" s="225"/>
+      <c r="D39" s="219"/>
+      <c r="E39" s="217"/>
+      <c r="F39" s="217" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B40" s="30"/>
-      <c r="C40" s="30"/>
-      <c r="D40" s="31"/>
-      <c r="E40" s="221"/>
-      <c r="F40" s="221" t="str">
+      <c r="B40" s="225"/>
+      <c r="C40" s="225"/>
+      <c r="D40" s="219"/>
+      <c r="E40" s="217"/>
+      <c r="F40" s="217" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="30"/>
-      <c r="C41" s="30"/>
-      <c r="D41" s="31"/>
-      <c r="E41" s="221"/>
-      <c r="F41" s="221" t="str">
+      <c r="B41" s="225"/>
+      <c r="C41" s="225"/>
+      <c r="D41" s="219"/>
+      <c r="E41" s="217"/>
+      <c r="F41" s="217" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B42" s="30"/>
-      <c r="C42" s="30"/>
-      <c r="D42" s="31"/>
-      <c r="E42" s="221"/>
-      <c r="F42" s="221" t="str">
+      <c r="B42" s="225"/>
+      <c r="C42" s="225"/>
+      <c r="D42" s="219"/>
+      <c r="E42" s="217"/>
+      <c r="F42" s="217" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B43" s="30"/>
-      <c r="C43" s="30"/>
-      <c r="D43" s="31"/>
-      <c r="E43" s="221"/>
-      <c r="F43" s="221" t="str">
+      <c r="B43" s="225"/>
+      <c r="C43" s="225"/>
+      <c r="D43" s="219"/>
+      <c r="E43" s="217"/>
+      <c r="F43" s="217" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>

</xml_diff>

<commit_message>
minor changes to presupuesto and to calc of portes in excel
</commit_message>
<xml_diff>
--- a/server/basePresupuestosExcel.xlsx
+++ b/server/basePresupuestosExcel.xlsx
@@ -2296,8 +2296,8 @@
   </sheetPr>
   <dimension ref="B3:J65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:F43"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2768,7 +2768,7 @@
         <v>0.33</v>
       </c>
       <c r="F47" s="35">
-        <f>D47*E47</f>
+        <f>IF(D47*E47&lt;17,17,D47*E47)</f>
         <v>62.7</v>
       </c>
     </row>

</xml_diff>